<commit_message>
Mockup calendarización y asignación a recursos
</commit_message>
<xml_diff>
--- a/tspi/ciclo-3/plan3-20106065.xlsx
+++ b/tspi/ciclo-3/plan3-20106065.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Configurar el repositorio local de la aplicación.</t>
+  </si>
+  <si>
+    <t>Actualizaciones al plan del proyecto</t>
   </si>
 </sst>
 </file>
@@ -644,7 +647,7 @@
   <dimension ref="A1:ALY23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -17423,7 +17426,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75"/>
@@ -17481,7 +17484,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="15">
-        <f t="shared" ref="F2:F7" si="0">((HOUR(D2)-HOUR(C2))*60)+(MINUTE(D2)-MINUTE(C2))-E2</f>
+        <f t="shared" ref="F2:F10" si="0">((HOUR(D2)-HOUR(C2))*60)+(MINUTE(D2)-MINUTE(C2))-E2</f>
         <v>27</v>
       </c>
       <c r="G2" s="20">
@@ -17624,28 +17627,82 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="26"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="26">
+        <v>41942</v>
+      </c>
+      <c r="B8" s="21">
+        <v>6</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="E8" s="21">
+        <v>20</v>
+      </c>
+      <c r="F8" s="15">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="27"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="21"/>
-      <c r="H9" s="9"/>
+      <c r="A9" s="27">
+        <v>41943</v>
+      </c>
+      <c r="B9" s="21">
+        <v>6</v>
+      </c>
+      <c r="C9" s="17">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0.36319444444444443</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0</v>
+      </c>
+      <c r="F9" s="15">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="G9" s="20">
+        <v>49</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="27"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="18"/>
-      <c r="H10" s="9"/>
+    <row r="10" spans="1:8" ht="25.5">
+      <c r="A10" s="27">
+        <v>41943</v>
+      </c>
+      <c r="B10" s="21">
+        <v>6</v>
+      </c>
+      <c r="C10" s="17">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D10" s="17">
+        <v>0.39166666666666666</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="G10" s="20">
+        <v>50</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="27"/>

</xml_diff>

<commit_message>
Versiones finales de los mockups
</commit_message>
<xml_diff>
--- a/tspi/ciclo-3/plan3-20106065.xlsx
+++ b/tspi/ciclo-3/plan3-20106065.xlsx
@@ -134,7 +134,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -160,6 +160,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -211,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -282,6 +288,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17426,7 +17433,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75"/>
@@ -17585,7 +17592,7 @@
       <c r="D6" s="17">
         <v>0.35972222222222222</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="32">
         <v>13</v>
       </c>
       <c r="F6" s="15">
@@ -17705,9 +17712,15 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="27"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="27">
+        <v>41944</v>
+      </c>
+      <c r="B11" s="21">
+        <v>6</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0.63958333333333328</v>
+      </c>
       <c r="D11" s="17"/>
       <c r="E11" s="21"/>
       <c r="F11" s="18"/>

</xml_diff>